<commit_message>
Quartz sync: Jun 5, 2025, 11:48 AM
</commit_message>
<xml_diff>
--- a/content/Resources/Key Resources.xlsx
+++ b/content/Resources/Key Resources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jderpak\OneDrive - North Okanagan-Shuswap School District 83\Personal\0 Queens 5+\JD Teacher Librarian Digital Portfolio\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sd83bcca-my.sharepoint.com/personal/jderpak_sd83_bc_ca/Documents/Personal/0 Queens 5+/tl-portfolio/content/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF76C2B-A4A1-4873-AA42-AE1B106A3410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{BEF76C2B-A4A1-4873-AA42-AE1B106A3410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF1D672A-FC25-44D1-AB4A-FEDDCBF48B1F}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{4E96F42E-F34F-41AB-A124-993A97A2BB54}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{4E96F42E-F34F-41AB-A124-993A97A2BB54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,15 +401,6 @@
   <dxfs count="7">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="8"/>
         <color rgb="FF333333"/>
         <name val="Arial"/>
@@ -470,6 +461,15 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="8"/>
         <color rgb="FF333333"/>
         <name val="Arial"/>
@@ -492,14 +492,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BBC6958-642D-4D39-B651-92B4822F3842}" name="Table1" displayName="Table1" ref="A1:E20" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BBC6958-642D-4D39-B651-92B4822F3842}" name="Table1" displayName="Table1" ref="A1:E20" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E20" xr:uid="{5BBC6958-642D-4D39-B651-92B4822F3842}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8778A8A5-309E-404C-96EE-2730C87C1A00}" name="MLA 9 Citation" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{C936C312-E8EC-45E6-A4E2-9427CCA44FF9}" name="Brief Description" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{9F13E2D4-5607-48D0-BA69-07AC895EB380}" name="Goal/Mission/Value of resource/Association/Author" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{12F09B72-BBF3-43D1-956B-68BE3218BF7D}" name="Pertinent Information" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{25598A92-72AC-48DF-B167-5644224655C6}" name="Other resources" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{8778A8A5-309E-404C-96EE-2730C87C1A00}" name="MLA 9 Citation" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{C936C312-E8EC-45E6-A4E2-9427CCA44FF9}" name="Brief Description" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{9F13E2D4-5607-48D0-BA69-07AC895EB380}" name="Goal/Mission/Value of resource/Association/Author" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{12F09B72-BBF3-43D1-956B-68BE3218BF7D}" name="Pertinent Information" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{25598A92-72AC-48DF-B167-5644224655C6}" name="Other resources" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -824,23 +824,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C28F015-54F8-4610-94E7-A7A4E483FACF}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B10" sqref="B10"/>
+      <selection pane="topRight" activeCell="B19" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -857,7 +857,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -874,7 +874,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="71.400000000000006" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -891,7 +891,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="102" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -908,7 +908,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -925,7 +925,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="124.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -942,7 +942,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -959,7 +959,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -976,7 +976,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="71.400000000000006" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -993,7 +993,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>91</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="142.80000000000001" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="101.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>92</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="71.400000000000006" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="71.400000000000006" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="71.400000000000006" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="71.400000000000006" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="71.400000000000006" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>